<commit_message>
feature(fonte-analise): refatora dados-painel-ldo com funcoes. Criação da base fonte-analise. see #11
</commit_message>
<xml_diff>
--- a/data/receita_analise.xlsx
+++ b/data/receita_analise.xlsx
@@ -1085,11 +1085,7 @@
           <t>1922990399000</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>60</v>
       </c>
@@ -1133,11 +1129,7 @@
           <t>1922990499000</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>60</v>
       </c>
@@ -1325,11 +1317,7 @@
           <t>1361012101000</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CESSAO DIR. OPERAC. PAG. - PODER JUDICIARIO - PRINC. - FOLHA DE PESSOAL</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>60</v>
       </c>
@@ -2077,11 +2065,7 @@
           <t>1741990133999</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>ACOES ESSENCIAIS JUSTICA - OUTROS</t>
-        </is>
-      </c>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
         <v>60</v>
       </c>
@@ -2173,11 +2157,7 @@
           <t>1921030101000</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>INDENIZACAO SINISTRO - PRINC.</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
         <v>60</v>
       </c>
@@ -4341,11 +4321,7 @@
           <t>1715520101000</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPLEM. UNIAO FUNDEB - VAAR - PRINC.</t>
-        </is>
-      </c>
+      <c r="D84" t="inlineStr"/>
       <c r="E84" t="n">
         <v>90</v>
       </c>
@@ -5061,11 +5037,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
         <v>13</v>
       </c>
@@ -5109,11 +5081,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D100" t="inlineStr"/>
       <c r="E100" t="n">
         <v>23</v>
       </c>
@@ -6261,11 +6229,7 @@
       <c r="E125" t="n">
         <v>79</v>
       </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F125" t="inlineStr"/>
       <c r="G125" t="n">
         <v>0</v>
       </c>
@@ -8205,11 +8169,7 @@
           <t>1741990140999</t>
         </is>
       </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>DESPORTO LAZER - OUTROS</t>
-        </is>
-      </c>
+      <c r="D167" t="inlineStr"/>
       <c r="E167" t="n">
         <v>59</v>
       </c>
@@ -11385,11 +11345,7 @@
           <t>1922063299000</t>
         </is>
       </c>
-      <c r="D234" t="inlineStr">
-        <is>
-          <t>RESTITUICAO DESPESAS PRIMARIAS EXERCICIOS ANTERIORES - MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D234" t="inlineStr"/>
       <c r="E234" t="n">
         <v>25</v>
       </c>
@@ -13449,11 +13405,7 @@
           <t>1219991206000</t>
         </is>
       </c>
-      <c r="D277" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - MJM - PECULIO</t>
-        </is>
-      </c>
+      <c r="D277" t="inlineStr"/>
       <c r="E277" t="n">
         <v>60</v>
       </c>
@@ -15417,11 +15369,7 @@
           <t>1999992116000</t>
         </is>
       </c>
-      <c r="D318" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - RENDAS DE LOTERIA CONVENCIONAL</t>
-        </is>
-      </c>
+      <c r="D318" t="inlineStr"/>
       <c r="E318" t="n">
         <v>60</v>
       </c>
@@ -15941,11 +15889,7 @@
           <t>1741990127999</t>
         </is>
       </c>
-      <c r="D329" t="inlineStr">
-        <is>
-          <t>EDUCACAO - OUTROS</t>
-        </is>
-      </c>
+      <c r="D329" t="inlineStr"/>
       <c r="E329" t="n">
         <v>45</v>
       </c>
@@ -17217,11 +17161,7 @@
           <t>1611010228000</t>
         </is>
       </c>
-      <c r="D356" t="inlineStr">
-        <is>
-          <t>SERVICOS ADM. COMERC. GER. - MJM - CONSULTORIA, ASSISTENCIA TECNICA E ANALISE DE PROJETOS</t>
-        </is>
-      </c>
+      <c r="D356" t="inlineStr"/>
       <c r="E356" t="n">
         <v>60</v>
       </c>
@@ -17417,11 +17357,7 @@
       <c r="E360" t="n">
         <v>79</v>
       </c>
-      <c r="F360" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F360" t="inlineStr"/>
       <c r="G360" t="n">
         <v>0</v>
       </c>
@@ -18585,11 +18521,7 @@
           <t>1349010301000</t>
         </is>
       </c>
-      <c r="D385" t="inlineStr">
-        <is>
-          <t>COMPENSACOES AMBIENTAIS - DA - REPOSICAO FLORESTAL</t>
-        </is>
-      </c>
+      <c r="D385" t="inlineStr"/>
       <c r="E385" t="n">
         <v>61</v>
       </c>
@@ -18633,11 +18565,7 @@
           <t>1349010401000</t>
         </is>
       </c>
-      <c r="D386" t="inlineStr">
-        <is>
-          <t>COMPENSACOES AMBIENTAIS - DA-MJM - REPOSICAO FLORESTAL</t>
-        </is>
-      </c>
+      <c r="D386" t="inlineStr"/>
       <c r="E386" t="n">
         <v>61</v>
       </c>
@@ -18929,11 +18857,7 @@
       <c r="E392" t="n">
         <v>79</v>
       </c>
-      <c r="F392" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F392" t="inlineStr"/>
       <c r="G392" t="n">
         <v>0</v>
       </c>
@@ -19305,11 +19229,7 @@
           <t>1215521102000</t>
         </is>
       </c>
-      <c r="D400" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D400" t="inlineStr"/>
       <c r="E400" t="n">
         <v>50</v>
       </c>
@@ -19353,11 +19273,7 @@
           <t>1215521103000</t>
         </is>
       </c>
-      <c r="D401" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D401" t="inlineStr"/>
       <c r="E401" t="n">
         <v>50</v>
       </c>
@@ -19401,11 +19317,7 @@
           <t>1215522102000</t>
         </is>
       </c>
-      <c r="D402" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D402" t="inlineStr"/>
       <c r="E402" t="n">
         <v>50</v>
       </c>
@@ -19449,11 +19361,7 @@
           <t>1215522103000</t>
         </is>
       </c>
-      <c r="D403" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D403" t="inlineStr"/>
       <c r="E403" t="n">
         <v>50</v>
       </c>
@@ -19593,11 +19501,7 @@
           <t>1219991103003</t>
         </is>
       </c>
-      <c r="D406" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A SAUDE - ATIVO</t>
-        </is>
-      </c>
+      <c r="D406" t="inlineStr"/>
       <c r="E406" t="n">
         <v>50</v>
       </c>
@@ -19641,11 +19545,7 @@
           <t>1219991103004</t>
         </is>
       </c>
-      <c r="D407" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A SAUDE - INATIVO</t>
-        </is>
-      </c>
+      <c r="D407" t="inlineStr"/>
       <c r="E407" t="n">
         <v>50</v>
       </c>
@@ -19689,11 +19589,7 @@
           <t>1219991103005</t>
         </is>
       </c>
-      <c r="D408" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A PREVIDENCIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D408" t="inlineStr"/>
       <c r="E408" t="n">
         <v>50</v>
       </c>
@@ -19737,11 +19633,7 @@
           <t>1219991103006</t>
         </is>
       </c>
-      <c r="D409" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A PREVIDENCIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D409" t="inlineStr"/>
       <c r="E409" t="n">
         <v>50</v>
       </c>
@@ -20457,11 +20349,7 @@
           <t>7215531101000</t>
         </is>
       </c>
-      <c r="D424" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D424" t="inlineStr"/>
       <c r="E424" t="n">
         <v>49</v>
       </c>
@@ -20505,11 +20393,7 @@
           <t>7215531102000</t>
         </is>
       </c>
-      <c r="D425" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D425" t="inlineStr"/>
       <c r="E425" t="n">
         <v>49</v>
       </c>
@@ -20553,11 +20437,7 @@
           <t>7215532101000</t>
         </is>
       </c>
-      <c r="D426" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D426" t="inlineStr"/>
       <c r="E426" t="n">
         <v>49</v>
       </c>
@@ -20601,11 +20481,7 @@
           <t>7215532102000</t>
         </is>
       </c>
-      <c r="D427" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D427" t="inlineStr"/>
       <c r="E427" t="n">
         <v>49</v>
       </c>
@@ -20745,11 +20621,7 @@
           <t>7219991103053</t>
         </is>
       </c>
-      <c r="D430" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A SAUDE - ATIVO</t>
-        </is>
-      </c>
+      <c r="D430" t="inlineStr"/>
       <c r="E430" t="n">
         <v>49</v>
       </c>
@@ -20793,11 +20665,7 @@
           <t>7219991103054</t>
         </is>
       </c>
-      <c r="D431" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A SAUDE - INATIVO</t>
-        </is>
-      </c>
+      <c r="D431" t="inlineStr"/>
       <c r="E431" t="n">
         <v>49</v>
       </c>
@@ -20841,11 +20709,7 @@
           <t>7219991103055</t>
         </is>
       </c>
-      <c r="D432" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A PREVIDENCIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D432" t="inlineStr"/>
       <c r="E432" t="n">
         <v>49</v>
       </c>
@@ -20889,11 +20753,7 @@
           <t>7219991103056</t>
         </is>
       </c>
-      <c r="D433" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A PREVIDENCIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D433" t="inlineStr"/>
       <c r="E433" t="n">
         <v>49</v>
       </c>
@@ -21881,11 +21741,7 @@
           <t>1761990139999</t>
         </is>
       </c>
-      <c r="D454" t="inlineStr">
-        <is>
-          <t>CULTURA - OUTROS</t>
-        </is>
-      </c>
+      <c r="D454" t="inlineStr"/>
       <c r="E454" t="n">
         <v>45</v>
       </c>
@@ -23113,11 +22969,7 @@
       <c r="E480" t="n">
         <v>79</v>
       </c>
-      <c r="F480" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F480" t="inlineStr"/>
       <c r="G480" t="n">
         <v>0</v>
       </c>
@@ -23393,11 +23245,7 @@
           <t>7121040104000</t>
         </is>
       </c>
-      <c r="D486" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - TX. CONTR. FISC. AMBIENT. - PRINC. - TAXA DE REGULARIZACAO AMBIENTAL</t>
-        </is>
-      </c>
+      <c r="D486" t="inlineStr"/>
       <c r="E486" t="n">
         <v>91</v>
       </c>
@@ -24157,11 +24005,7 @@
           <t>1351010101000</t>
         </is>
       </c>
-      <c r="D502" t="inlineStr">
-        <is>
-          <t>OUTORGA DIR. USO EXPLORACAO CRIACAO PROTEGIDA - INSTITUICAO CIENTIFICA TECNOLOGICA - PRINC.</t>
-        </is>
-      </c>
+      <c r="D502" t="inlineStr"/>
       <c r="E502" t="n">
         <v>60</v>
       </c>
@@ -25721,11 +25565,7 @@
           <t>1923990103000</t>
         </is>
       </c>
-      <c r="D535" t="inlineStr">
-        <is>
-          <t>OUTROS RESSARCIMENTOS - PRINC. - FORMACAO ACADEMICA NA AREA DE SAUDE</t>
-        </is>
-      </c>
+      <c r="D535" t="inlineStr"/>
       <c r="E535" t="n">
         <v>60</v>
       </c>
@@ -28261,11 +28101,7 @@
           <t>1351010101000</t>
         </is>
       </c>
-      <c r="D589" t="inlineStr">
-        <is>
-          <t>OUTORGA DIR. USO EXPLORACAO CRIACAO PROTEGIDA - INSTITUICAO CIENTIFICA TECNOLOGICA - PRINC.</t>
-        </is>
-      </c>
+      <c r="D589" t="inlineStr"/>
       <c r="E589" t="n">
         <v>60</v>
       </c>
@@ -28549,11 +28385,7 @@
           <t>1631530201000</t>
         </is>
       </c>
-      <c r="D595" t="inlineStr">
-        <is>
-          <t>SERVICOS AMBULATORIAIS - MJM</t>
-        </is>
-      </c>
+      <c r="D595" t="inlineStr"/>
       <c r="E595" t="n">
         <v>60</v>
       </c>
@@ -32425,11 +32257,7 @@
           <t>7699990101000</t>
         </is>
       </c>
-      <c r="D677" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - OUTROS SERVICOS - PRINC.</t>
-        </is>
-      </c>
+      <c r="D677" t="inlineStr"/>
       <c r="E677" t="n">
         <v>60</v>
       </c>
@@ -32845,11 +32673,7 @@
           <t>1611010129000</t>
         </is>
       </c>
-      <c r="D686" t="inlineStr">
-        <is>
-          <t>SERVICOS ADM. COMERC. GER. - PRINC. - HOSPEDAGEM E ALIMENTACAO</t>
-        </is>
-      </c>
+      <c r="D686" t="inlineStr"/>
       <c r="E686" t="n">
         <v>60</v>
       </c>
@@ -35333,11 +35157,7 @@
           <t>1911090499000</t>
         </is>
       </c>
-      <c r="D738" t="inlineStr">
-        <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D738" t="inlineStr"/>
       <c r="E738" t="n">
         <v>60</v>
       </c>
@@ -35381,11 +35201,7 @@
           <t>1911090499000</t>
         </is>
       </c>
-      <c r="D739" t="inlineStr">
-        <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D739" t="inlineStr"/>
       <c r="E739" t="n">
         <v>77</v>
       </c>
@@ -36055,7 +35871,7 @@
       </c>
       <c r="D753" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E753" t="n">
@@ -36477,7 +36293,7 @@
       </c>
       <c r="B762" t="inlineStr">
         <is>
-          <t>FUNDALEMG</t>
+          <t>FUNDHAB</t>
         </is>
       </c>
       <c r="C762" t="inlineStr">
@@ -36525,7 +36341,7 @@
       </c>
       <c r="B763" t="inlineStr">
         <is>
-          <t>FUNDALEMG</t>
+          <t>FUNDHAB</t>
         </is>
       </c>
       <c r="C763" t="inlineStr">
@@ -36573,7 +36389,7 @@
       </c>
       <c r="B764" t="inlineStr">
         <is>
-          <t>FUNDALEMG</t>
+          <t>FUNDHAB</t>
         </is>
       </c>
       <c r="C764" t="inlineStr">
@@ -37721,11 +37537,7 @@
           <t>1739990111001</t>
         </is>
       </c>
-      <c r="D789" t="inlineStr">
-        <is>
-          <t>COMERCIO E SERVICOS - DIVERSOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D789" t="inlineStr"/>
       <c r="E789" t="n">
         <v>59</v>
       </c>
@@ -38201,11 +38013,7 @@
           <t>1611030105000</t>
         </is>
       </c>
-      <c r="D799" t="inlineStr">
-        <is>
-          <t>SERVICOS REG. CERTIF. FISCALIZ. - PRINC. - INSPECAO E FISCALIZACAO</t>
-        </is>
-      </c>
+      <c r="D799" t="inlineStr"/>
       <c r="E799" t="n">
         <v>60</v>
       </c>
@@ -39305,11 +39113,7 @@
           <t>7729990127000</t>
         </is>
       </c>
-      <c r="D822" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - OUTRAS TRANSF. ESTADOS DF - PRINC. - REPASSE DO FUNDO ESPECIAL DO MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - FUNEMP</t>
-        </is>
-      </c>
+      <c r="D822" t="inlineStr"/>
       <c r="E822" t="n">
         <v>60</v>
       </c>
@@ -39835,7 +39639,7 @@
       </c>
       <c r="D833" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E833" t="n">
@@ -40361,11 +40165,7 @@
           <t>1321050101000</t>
         </is>
       </c>
-      <c r="D844" t="inlineStr">
-        <is>
-          <t>JUROS TITULOS RENDA - PRINC. - RENDIMENTO DE APLICACAO FINANCEIRA - TITULOS DE CREDITO</t>
-        </is>
-      </c>
+      <c r="D844" t="inlineStr"/>
       <c r="E844" t="n">
         <v>60</v>
       </c>
@@ -40553,11 +40353,7 @@
           <t>1911090101003</t>
         </is>
       </c>
-      <c r="D848" t="inlineStr">
-        <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - PRINC. - PPP - DIREITOS DA CIDADANIA</t>
-        </is>
-      </c>
+      <c r="D848" t="inlineStr"/>
       <c r="E848" t="n">
         <v>60</v>
       </c>
@@ -41889,11 +41685,7 @@
           <t>1219991110001</t>
         </is>
       </c>
-      <c r="D876" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D876" t="inlineStr"/>
       <c r="E876" t="n">
         <v>30</v>
       </c>
@@ -42753,11 +42545,7 @@
           <t>7219991110051</t>
         </is>
       </c>
-      <c r="D894" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D894" t="inlineStr"/>
       <c r="E894" t="n">
         <v>75</v>
       </c>
@@ -42801,11 +42589,7 @@
           <t>7219991110052</t>
         </is>
       </c>
-      <c r="D895" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D895" t="inlineStr"/>
       <c r="E895" t="n">
         <v>75</v>
       </c>
@@ -43045,11 +42829,7 @@
           <t>1999122101000</t>
         </is>
       </c>
-      <c r="D901" t="inlineStr">
-        <is>
-          <t>ONUS SUCUMBENCIA - PRINC. - HONORARIOS DE ADVOGADOS</t>
-        </is>
-      </c>
+      <c r="D901" t="inlineStr"/>
       <c r="E901" t="n">
         <v>60</v>
       </c>
@@ -44909,11 +44689,7 @@
           <t>1114501101002</t>
         </is>
       </c>
-      <c r="D942" t="inlineStr">
-        <is>
-          <t>ICMS - PRINC. - COTA PARTE ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D942" t="inlineStr"/>
       <c r="E942" t="n">
         <v>10</v>
       </c>
@@ -45101,11 +44877,7 @@
           <t>1114501201002</t>
         </is>
       </c>
-      <c r="D946" t="inlineStr">
-        <is>
-          <t>ICMS - MJM - COTA PARTE ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D946" t="inlineStr"/>
       <c r="E946" t="n">
         <v>10</v>
       </c>
@@ -47213,11 +46985,7 @@
           <t>1121010301002</t>
         </is>
       </c>
-      <c r="D990" t="inlineStr">
-        <is>
-          <t>TX. INSP. CONTR. FISC. - DA - TX. SEGURANCA PUBLICA - CORPO DE BOMBEIROS MILITAR DO ESTADO DE MINAS GERAIS - CBMMG</t>
-        </is>
-      </c>
+      <c r="D990" t="inlineStr"/>
       <c r="E990" t="n">
         <v>27</v>
       </c>
@@ -47453,11 +47221,7 @@
           <t>1121010401002</t>
         </is>
       </c>
-      <c r="D995" t="inlineStr">
-        <is>
-          <t>TX. INSP. CONTR. FISC. - DA-MJM - TX. SEGURANCA PUBLICA - CORPO DE BOMBEIROS MILITAR DO ESTADO DE MINAS GERAIS - CBMMG</t>
-        </is>
-      </c>
+      <c r="D995" t="inlineStr"/>
       <c r="E995" t="n">
         <v>27</v>
       </c>
@@ -49949,11 +49713,7 @@
           <t>1215521101000</t>
         </is>
       </c>
-      <c r="D1047" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - APOSENTADORIA</t>
-        </is>
-      </c>
+      <c r="D1047" t="inlineStr"/>
       <c r="E1047" t="n">
         <v>30</v>
       </c>
@@ -50141,11 +49901,7 @@
           <t>1219991110001</t>
         </is>
       </c>
-      <c r="D1051" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D1051" t="inlineStr"/>
       <c r="E1051" t="n">
         <v>30</v>
       </c>
@@ -50573,11 +50329,7 @@
           <t>1311020102000</t>
         </is>
       </c>
-      <c r="D1060" t="inlineStr">
-        <is>
-          <t>CONC. PERM. AUTOR. CESSAO DIR. USO BENS IMOV. PUB. - PRINC. - CESSAO DO DIREITO DE EXPLORACAO DE ESTADIOS - ARENA INDEPENDENCIA</t>
-        </is>
-      </c>
+      <c r="D1060" t="inlineStr"/>
       <c r="E1060" t="n">
         <v>15</v>
       </c>
@@ -50813,11 +50565,7 @@
           <t>1311990101000</t>
         </is>
       </c>
-      <c r="D1065" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. IMOBILIARIAS - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1065" t="inlineStr"/>
       <c r="E1065" t="n">
         <v>15</v>
       </c>
@@ -50861,11 +50609,7 @@
           <t>1311990201000</t>
         </is>
       </c>
-      <c r="D1066" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. IMOBILIARIAS - MJM</t>
-        </is>
-      </c>
+      <c r="D1066" t="inlineStr"/>
       <c r="E1066" t="n">
         <v>15</v>
       </c>
@@ -51917,11 +51661,7 @@
           <t>1321020101000</t>
         </is>
       </c>
-      <c r="D1088" t="inlineStr">
-        <is>
-          <t>REMUNERACAO DEPOSITOS ESPECIAIS - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1088" t="inlineStr"/>
       <c r="E1088" t="n">
         <v>15</v>
       </c>
@@ -51965,11 +51705,7 @@
           <t>1321050102000</t>
         </is>
       </c>
-      <c r="D1089" t="inlineStr">
-        <is>
-          <t>JUROS TITULOS RENDA - PRINC. - RENDIMENTO FINANCEIRO - ATIVO BDMG/CREDIREAL/BEMGE - SANEAMENTO SISTEMA FINANCEIRO</t>
-        </is>
-      </c>
+      <c r="D1089" t="inlineStr"/>
       <c r="E1089" t="n">
         <v>15</v>
       </c>
@@ -52637,11 +52373,7 @@
           <t>1361012101000</t>
         </is>
       </c>
-      <c r="D1103" t="inlineStr">
-        <is>
-          <t>CESSAO DIR. OPERAC. PAG. - PODER JUDICIARIO - PRINC. - FOLHA DE PESSOAL</t>
-        </is>
-      </c>
+      <c r="D1103" t="inlineStr"/>
       <c r="E1103" t="n">
         <v>60</v>
       </c>
@@ -53933,11 +53665,7 @@
           <t>1611010135000</t>
         </is>
       </c>
-      <c r="D1130" t="inlineStr">
-        <is>
-          <t>SERVICOS ADM. COMERC. GER. - PRINC. - REGISTRO ELETRONICO DE CONTRATO INTEGRAL</t>
-        </is>
-      </c>
+      <c r="D1130" t="inlineStr"/>
       <c r="E1130" t="n">
         <v>15</v>
       </c>
@@ -55229,11 +54957,7 @@
           <t>1715520101000</t>
         </is>
       </c>
-      <c r="D1157" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPLEM. UNIAO FUNDEB - VAAR - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1157" t="inlineStr"/>
       <c r="E1157" t="n">
         <v>90</v>
       </c>
@@ -55325,11 +55049,7 @@
           <t>1719620101000</t>
         </is>
       </c>
-      <c r="D1159" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO ESTADO</t>
-        </is>
-      </c>
+      <c r="D1159" t="inlineStr"/>
       <c r="E1159" t="n">
         <v>19</v>
       </c>
@@ -55373,11 +55093,7 @@
           <t>1719620102000</t>
         </is>
       </c>
-      <c r="D1160" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D1160" t="inlineStr"/>
       <c r="E1160" t="n">
         <v>20</v>
       </c>
@@ -55421,11 +55137,7 @@
           <t>1719620103000</t>
         </is>
       </c>
-      <c r="D1161" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
-        </is>
-      </c>
+      <c r="D1161" t="inlineStr"/>
       <c r="E1161" t="n">
         <v>23</v>
       </c>
@@ -55517,11 +55229,7 @@
           <t>1719990129000</t>
         </is>
       </c>
-      <c r="D1163" t="inlineStr">
-        <is>
-          <t>OUTRAS TRANSF. UNIAO ENTIDADES - AUXILIO DE COMPLEMENTACAO DO FPE - LC N 201/2023</t>
-        </is>
-      </c>
+      <c r="D1163" t="inlineStr"/>
       <c r="E1163" t="n">
         <v>15</v>
       </c>
@@ -55565,11 +55273,7 @@
           <t>1739990111001</t>
         </is>
       </c>
-      <c r="D1164" t="inlineStr">
-        <is>
-          <t>COMERCIO E SERVICOS - DIVERSOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D1164" t="inlineStr"/>
       <c r="E1164" t="n">
         <v>11</v>
       </c>
@@ -55613,11 +55317,7 @@
           <t>1741990133999</t>
         </is>
       </c>
-      <c r="D1165" t="inlineStr">
-        <is>
-          <t>ACOES ESSENCIAIS JUSTICA - OUTROS</t>
-        </is>
-      </c>
+      <c r="D1165" t="inlineStr"/>
       <c r="E1165" t="n">
         <v>60</v>
       </c>
@@ -55757,11 +55457,7 @@
           <t>1741990140999</t>
         </is>
       </c>
-      <c r="D1168" t="inlineStr">
-        <is>
-          <t>DESPORTO LAZER - OUTROS</t>
-        </is>
-      </c>
+      <c r="D1168" t="inlineStr"/>
       <c r="E1168" t="n">
         <v>11</v>
       </c>
@@ -55805,11 +55501,7 @@
           <t>1741990140999</t>
         </is>
       </c>
-      <c r="D1169" t="inlineStr">
-        <is>
-          <t>DESPORTO LAZER - OUTROS</t>
-        </is>
-      </c>
+      <c r="D1169" t="inlineStr"/>
       <c r="E1169" t="n">
         <v>59</v>
       </c>
@@ -55855,7 +55547,7 @@
       </c>
       <c r="D1170" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E1170" t="n">
@@ -55903,7 +55595,7 @@
       </c>
       <c r="D1171" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E1171" t="n">
@@ -55951,7 +55643,7 @@
       </c>
       <c r="D1172" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E1172" t="n">
@@ -56093,11 +55785,7 @@
           <t>1751500102001</t>
         </is>
       </c>
-      <c r="D1175" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - LC FEDERAL NO 87/96 - COTA PARTE DO ESTADO</t>
-        </is>
-      </c>
+      <c r="D1175" t="inlineStr"/>
       <c r="E1175" t="n">
         <v>23</v>
       </c>
@@ -56765,11 +56453,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D1189" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D1189" t="inlineStr"/>
       <c r="E1189" t="n">
         <v>13</v>
       </c>
@@ -56813,11 +56497,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D1190" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D1190" t="inlineStr"/>
       <c r="E1190" t="n">
         <v>23</v>
       </c>
@@ -56957,11 +56637,7 @@
           <t>1792010101000</t>
         </is>
       </c>
-      <c r="D1193" t="inlineStr">
-        <is>
-          <t>TRANSF. DEPOSITOS NAO IDENTIFICADOS - PRINC. - CAMPANHA DE DOACAO CORONAVIRUS</t>
-        </is>
-      </c>
+      <c r="D1193" t="inlineStr"/>
       <c r="E1193" t="n">
         <v>26</v>
       </c>
@@ -57005,11 +56681,7 @@
           <t>1792010101000</t>
         </is>
       </c>
-      <c r="D1194" t="inlineStr">
-        <is>
-          <t>TRANSF. DEPOSITOS NAO IDENTIFICADOS - PRINC. - CAMPANHA DE DOACAO CORONAVIRUS</t>
-        </is>
-      </c>
+      <c r="D1194" t="inlineStr"/>
       <c r="E1194" t="n">
         <v>46</v>
       </c>
@@ -57341,11 +57013,7 @@
           <t>1911010104001</t>
         </is>
       </c>
-      <c r="D1201" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1201" t="inlineStr"/>
       <c r="E1201" t="n">
         <v>15</v>
       </c>
@@ -57533,11 +57201,7 @@
           <t>1911010109000</t>
         </is>
       </c>
-      <c r="D1205" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - DESMONTE DE VEICULOS</t>
-        </is>
-      </c>
+      <c r="D1205" t="inlineStr"/>
       <c r="E1205" t="n">
         <v>15</v>
       </c>
@@ -57725,11 +57389,7 @@
           <t>1911010304001</t>
         </is>
       </c>
-      <c r="D1209" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISL. ESPECIFICA - DA - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1209" t="inlineStr"/>
       <c r="E1209" t="n">
         <v>15</v>
       </c>
@@ -57973,11 +57633,7 @@
       <c r="E1214" t="n">
         <v>79</v>
       </c>
-      <c r="F1214" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F1214" t="inlineStr"/>
       <c r="G1214" t="n">
         <v>0</v>
       </c>
@@ -58205,11 +57861,7 @@
           <t>1911132101000</t>
         </is>
       </c>
-      <c r="D1219" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISLACAO ANTICORRUPCAO ACORDOS LENIENCIA - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1219" t="inlineStr"/>
       <c r="E1219" t="n">
         <v>15</v>
       </c>
@@ -58349,11 +58001,7 @@
           <t>1921030101000</t>
         </is>
       </c>
-      <c r="D1222" t="inlineStr">
-        <is>
-          <t>INDENIZACAO SINISTRO - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1222" t="inlineStr"/>
       <c r="E1222" t="n">
         <v>60</v>
       </c>
@@ -59021,11 +58669,7 @@
           <t>1922063299000</t>
         </is>
       </c>
-      <c r="D1236" t="inlineStr">
-        <is>
-          <t>RESTITUICAO DESPESAS PRIMARIAS EXERCICIOS ANTERIORES - MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D1236" t="inlineStr"/>
       <c r="E1236" t="n">
         <v>25</v>
       </c>
@@ -60029,11 +59673,7 @@
           <t>1922990399000</t>
         </is>
       </c>
-      <c r="D1257" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D1257" t="inlineStr"/>
       <c r="E1257" t="n">
         <v>60</v>
       </c>
@@ -60077,11 +59717,7 @@
           <t>1922990499000</t>
         </is>
       </c>
-      <c r="D1258" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D1258" t="inlineStr"/>
       <c r="E1258" t="n">
         <v>60</v>
       </c>
@@ -60365,11 +60001,7 @@
           <t>1999992101000</t>
         </is>
       </c>
-      <c r="D1264" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - RECURSOS DE DEPOSITOS JUDICIAIS</t>
-        </is>
-      </c>
+      <c r="D1264" t="inlineStr"/>
       <c r="E1264" t="n">
         <v>23</v>
       </c>
@@ -60605,11 +60237,7 @@
           <t>1999992113000</t>
         </is>
       </c>
-      <c r="D1269" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - CONVERSAO EM RENDA DE VALORES PENHORADOS EM ACOES JUDICIAIS</t>
-        </is>
-      </c>
+      <c r="D1269" t="inlineStr"/>
       <c r="E1269" t="n">
         <v>15</v>
       </c>
@@ -61373,11 +61001,7 @@
           <t>2211020104000</t>
         </is>
       </c>
-      <c r="D1285" t="inlineStr">
-        <is>
-          <t>ALIEN. TITULOS VALORES MOBIL. APLIC. CONGEN. PERMANENTES - PRINC. - MINAS CAIXA</t>
-        </is>
-      </c>
+      <c r="D1285" t="inlineStr"/>
       <c r="E1285" t="n">
         <v>48</v>
       </c>
@@ -61421,11 +61045,7 @@
           <t>2211020105000</t>
         </is>
       </c>
-      <c r="D1286" t="inlineStr">
-        <is>
-          <t>ALIEN. TITULOS VALORES MOBIL. APLIC. CONGEN. PERMANENTES - PRINC. - SANEAMENTO DO SISTEMA FINANCEIRO - CREDIREAL/BEMGE</t>
-        </is>
-      </c>
+      <c r="D1286" t="inlineStr"/>
       <c r="E1286" t="n">
         <v>48</v>
       </c>
@@ -61999,7 +61619,7 @@
       </c>
       <c r="D1298" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - DEMAIS RECURSOS</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
         </is>
       </c>
       <c r="E1298" t="n">
@@ -62045,11 +61665,7 @@
           <t>2999990104000</t>
         </is>
       </c>
-      <c r="D1299" t="inlineStr">
-        <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - ACORDO JUDICIAL DE REPARACAO INTEGRAL E DEFINITIVA</t>
-        </is>
-      </c>
+      <c r="D1299" t="inlineStr"/>
       <c r="E1299" t="n">
         <v>80</v>
       </c>
@@ -62093,11 +61709,7 @@
           <t>7215531102000</t>
         </is>
       </c>
-      <c r="D1300" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D1300" t="inlineStr"/>
       <c r="E1300" t="n">
         <v>75</v>
       </c>
@@ -62141,11 +61753,7 @@
           <t>7215531103000</t>
         </is>
       </c>
-      <c r="D1301" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - APOSENTADORIA</t>
-        </is>
-      </c>
+      <c r="D1301" t="inlineStr"/>
       <c r="E1301" t="n">
         <v>75</v>
       </c>
@@ -62189,11 +61797,7 @@
           <t>7215532102000</t>
         </is>
       </c>
-      <c r="D1302" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D1302" t="inlineStr"/>
       <c r="E1302" t="n">
         <v>75</v>
       </c>
@@ -62237,11 +61841,7 @@
           <t>7215532103000</t>
         </is>
       </c>
-      <c r="D1303" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - APOSENTADORIA</t>
-        </is>
-      </c>
+      <c r="D1303" t="inlineStr"/>
       <c r="E1303" t="n">
         <v>75</v>
       </c>
@@ -62285,11 +61885,7 @@
           <t>7219991110051</t>
         </is>
       </c>
-      <c r="D1304" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D1304" t="inlineStr"/>
       <c r="E1304" t="n">
         <v>75</v>
       </c>
@@ -62333,11 +61929,7 @@
           <t>7219991110052</t>
         </is>
       </c>
-      <c r="D1305" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D1305" t="inlineStr"/>
       <c r="E1305" t="n">
         <v>75</v>
       </c>
@@ -62957,11 +62549,7 @@
           <t>9114501101002</t>
         </is>
       </c>
-      <c r="D1318" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DO ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1318" t="inlineStr"/>
       <c r="E1318" t="n">
         <v>10</v>
       </c>
@@ -63101,11 +62689,7 @@
           <t>9114501201002</t>
         </is>
       </c>
-      <c r="D1321" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DO ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1321" t="inlineStr"/>
       <c r="E1321" t="n">
         <v>10</v>
       </c>
@@ -63773,11 +63357,7 @@
           <t>9719620102000</t>
         </is>
       </c>
-      <c r="D1335" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D1335" t="inlineStr"/>
       <c r="E1335" t="n">
         <v>20</v>
       </c>
@@ -63821,11 +63401,7 @@
           <t>9719620103000</t>
         </is>
       </c>
-      <c r="D1336" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
-        </is>
-      </c>
+      <c r="D1336" t="inlineStr"/>
       <c r="E1336" t="n">
         <v>23</v>
       </c>
@@ -63965,11 +63541,7 @@
           <t>9911010104001</t>
         </is>
       </c>
-      <c r="D1339" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - MULTAS LEGISL. ESPECIFICA - PRINC. - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1339" t="inlineStr"/>
       <c r="E1339" t="n">
         <v>15</v>
       </c>
@@ -64013,11 +63585,7 @@
           <t>9911010304001</t>
         </is>
       </c>
-      <c r="D1340" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - MULTAS LEGISL. ESPECIFICA - DA - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1340" t="inlineStr"/>
       <c r="E1340" t="n">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Base agregada ano-uo-fonte (#12)
* feature(fonte-analise): refatora código e implementa base de análise agregada por ano-uo-fonte

---------

Authored-by: labanca <moraislabanca@gmail.com>
Co-authored-by:  carloshob
</commit_message>
<xml_diff>
--- a/data/receita_analise.xlsx
+++ b/data/receita_analise.xlsx
@@ -1085,11 +1085,7 @@
           <t>1922990399000</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>60</v>
       </c>
@@ -1133,11 +1129,7 @@
           <t>1922990499000</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>60</v>
       </c>
@@ -1325,11 +1317,7 @@
           <t>1361012101000</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>CESSAO DIR. OPERAC. PAG. - PODER JUDICIARIO - PRINC. - FOLHA DE PESSOAL</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>60</v>
       </c>
@@ -2077,11 +2065,7 @@
           <t>1741990133999</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>ACOES ESSENCIAIS JUSTICA - OUTROS</t>
-        </is>
-      </c>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
         <v>60</v>
       </c>
@@ -2173,11 +2157,7 @@
           <t>1921030101000</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>INDENIZACAO SINISTRO - PRINC.</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
         <v>60</v>
       </c>
@@ -4341,11 +4321,7 @@
           <t>1715520101000</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPLEM. UNIAO FUNDEB - VAAR - PRINC.</t>
-        </is>
-      </c>
+      <c r="D84" t="inlineStr"/>
       <c r="E84" t="n">
         <v>90</v>
       </c>
@@ -5061,11 +5037,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
         <v>13</v>
       </c>
@@ -5109,11 +5081,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D100" t="inlineStr"/>
       <c r="E100" t="n">
         <v>23</v>
       </c>
@@ -6261,11 +6229,7 @@
       <c r="E125" t="n">
         <v>79</v>
       </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F125" t="inlineStr"/>
       <c r="G125" t="n">
         <v>0</v>
       </c>
@@ -8205,11 +8169,7 @@
           <t>1741990140999</t>
         </is>
       </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>DESPORTO LAZER - OUTROS</t>
-        </is>
-      </c>
+      <c r="D167" t="inlineStr"/>
       <c r="E167" t="n">
         <v>59</v>
       </c>
@@ -11385,11 +11345,7 @@
           <t>1922063299000</t>
         </is>
       </c>
-      <c r="D234" t="inlineStr">
-        <is>
-          <t>RESTITUICAO DESPESAS PRIMARIAS EXERCICIOS ANTERIORES - MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D234" t="inlineStr"/>
       <c r="E234" t="n">
         <v>25</v>
       </c>
@@ -13449,11 +13405,7 @@
           <t>1219991206000</t>
         </is>
       </c>
-      <c r="D277" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - MJM - PECULIO</t>
-        </is>
-      </c>
+      <c r="D277" t="inlineStr"/>
       <c r="E277" t="n">
         <v>60</v>
       </c>
@@ -15417,11 +15369,7 @@
           <t>1999992116000</t>
         </is>
       </c>
-      <c r="D318" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - RENDAS DE LOTERIA CONVENCIONAL</t>
-        </is>
-      </c>
+      <c r="D318" t="inlineStr"/>
       <c r="E318" t="n">
         <v>60</v>
       </c>
@@ -15941,11 +15889,7 @@
           <t>1741990127999</t>
         </is>
       </c>
-      <c r="D329" t="inlineStr">
-        <is>
-          <t>EDUCACAO - OUTROS</t>
-        </is>
-      </c>
+      <c r="D329" t="inlineStr"/>
       <c r="E329" t="n">
         <v>45</v>
       </c>
@@ -17217,11 +17161,7 @@
           <t>1611010228000</t>
         </is>
       </c>
-      <c r="D356" t="inlineStr">
-        <is>
-          <t>SERVICOS ADM. COMERC. GER. - MJM - CONSULTORIA, ASSISTENCIA TECNICA E ANALISE DE PROJETOS</t>
-        </is>
-      </c>
+      <c r="D356" t="inlineStr"/>
       <c r="E356" t="n">
         <v>60</v>
       </c>
@@ -17417,11 +17357,7 @@
       <c r="E360" t="n">
         <v>79</v>
       </c>
-      <c r="F360" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F360" t="inlineStr"/>
       <c r="G360" t="n">
         <v>0</v>
       </c>
@@ -18585,11 +18521,7 @@
           <t>1349010301000</t>
         </is>
       </c>
-      <c r="D385" t="inlineStr">
-        <is>
-          <t>COMPENSACOES AMBIENTAIS - DA - REPOSICAO FLORESTAL</t>
-        </is>
-      </c>
+      <c r="D385" t="inlineStr"/>
       <c r="E385" t="n">
         <v>61</v>
       </c>
@@ -18633,11 +18565,7 @@
           <t>1349010401000</t>
         </is>
       </c>
-      <c r="D386" t="inlineStr">
-        <is>
-          <t>COMPENSACOES AMBIENTAIS - DA-MJM - REPOSICAO FLORESTAL</t>
-        </is>
-      </c>
+      <c r="D386" t="inlineStr"/>
       <c r="E386" t="n">
         <v>61</v>
       </c>
@@ -18929,11 +18857,7 @@
       <c r="E392" t="n">
         <v>79</v>
       </c>
-      <c r="F392" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F392" t="inlineStr"/>
       <c r="G392" t="n">
         <v>0</v>
       </c>
@@ -19305,11 +19229,7 @@
           <t>1215521102000</t>
         </is>
       </c>
-      <c r="D400" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D400" t="inlineStr"/>
       <c r="E400" t="n">
         <v>50</v>
       </c>
@@ -19353,11 +19273,7 @@
           <t>1215521103000</t>
         </is>
       </c>
-      <c r="D401" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D401" t="inlineStr"/>
       <c r="E401" t="n">
         <v>50</v>
       </c>
@@ -19401,11 +19317,7 @@
           <t>1215522102000</t>
         </is>
       </c>
-      <c r="D402" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D402" t="inlineStr"/>
       <c r="E402" t="n">
         <v>50</v>
       </c>
@@ -19449,11 +19361,7 @@
           <t>1215522103000</t>
         </is>
       </c>
-      <c r="D403" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D403" t="inlineStr"/>
       <c r="E403" t="n">
         <v>50</v>
       </c>
@@ -19593,11 +19501,7 @@
           <t>1219991103003</t>
         </is>
       </c>
-      <c r="D406" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A SAUDE - ATIVO</t>
-        </is>
-      </c>
+      <c r="D406" t="inlineStr"/>
       <c r="E406" t="n">
         <v>50</v>
       </c>
@@ -19641,11 +19545,7 @@
           <t>1219991103004</t>
         </is>
       </c>
-      <c r="D407" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A SAUDE - INATIVO</t>
-        </is>
-      </c>
+      <c r="D407" t="inlineStr"/>
       <c r="E407" t="n">
         <v>50</v>
       </c>
@@ -19689,11 +19589,7 @@
           <t>1219991103005</t>
         </is>
       </c>
-      <c r="D408" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A PREVIDENCIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D408" t="inlineStr"/>
       <c r="E408" t="n">
         <v>50</v>
       </c>
@@ -19737,11 +19633,7 @@
           <t>1219991103006</t>
         </is>
       </c>
-      <c r="D409" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. MILITAR PARA A PREVIDENCIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D409" t="inlineStr"/>
       <c r="E409" t="n">
         <v>50</v>
       </c>
@@ -20457,11 +20349,7 @@
           <t>7215531101000</t>
         </is>
       </c>
-      <c r="D424" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D424" t="inlineStr"/>
       <c r="E424" t="n">
         <v>49</v>
       </c>
@@ -20505,11 +20393,7 @@
           <t>7215531102000</t>
         </is>
       </c>
-      <c r="D425" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D425" t="inlineStr"/>
       <c r="E425" t="n">
         <v>49</v>
       </c>
@@ -20553,11 +20437,7 @@
           <t>7215532101000</t>
         </is>
       </c>
-      <c r="D426" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - SAUDE</t>
-        </is>
-      </c>
+      <c r="D426" t="inlineStr"/>
       <c r="E426" t="n">
         <v>49</v>
       </c>
@@ -20601,11 +20481,7 @@
           <t>7215532102000</t>
         </is>
       </c>
-      <c r="D427" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D427" t="inlineStr"/>
       <c r="E427" t="n">
         <v>49</v>
       </c>
@@ -20745,11 +20621,7 @@
           <t>7219991103053</t>
         </is>
       </c>
-      <c r="D430" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A SAUDE - ATIVO</t>
-        </is>
-      </c>
+      <c r="D430" t="inlineStr"/>
       <c r="E430" t="n">
         <v>49</v>
       </c>
@@ -20793,11 +20665,7 @@
           <t>7219991103054</t>
         </is>
       </c>
-      <c r="D431" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A SAUDE - INATIVO</t>
-        </is>
-      </c>
+      <c r="D431" t="inlineStr"/>
       <c r="E431" t="n">
         <v>49</v>
       </c>
@@ -20841,11 +20709,7 @@
           <t>7219991103055</t>
         </is>
       </c>
-      <c r="D432" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A PREVIDENCIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D432" t="inlineStr"/>
       <c r="E432" t="n">
         <v>49</v>
       </c>
@@ -20889,11 +20753,7 @@
           <t>7219991103056</t>
         </is>
       </c>
-      <c r="D433" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL MILITAR PARA A PREVIDENCIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D433" t="inlineStr"/>
       <c r="E433" t="n">
         <v>49</v>
       </c>
@@ -21881,11 +21741,7 @@
           <t>1761990139999</t>
         </is>
       </c>
-      <c r="D454" t="inlineStr">
-        <is>
-          <t>CULTURA - OUTROS</t>
-        </is>
-      </c>
+      <c r="D454" t="inlineStr"/>
       <c r="E454" t="n">
         <v>45</v>
       </c>
@@ -23113,11 +22969,7 @@
       <c r="E480" t="n">
         <v>79</v>
       </c>
-      <c r="F480" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F480" t="inlineStr"/>
       <c r="G480" t="n">
         <v>0</v>
       </c>
@@ -23393,11 +23245,7 @@
           <t>7121040104000</t>
         </is>
       </c>
-      <c r="D486" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - TX. CONTR. FISC. AMBIENT. - PRINC. - TAXA DE REGULARIZACAO AMBIENTAL</t>
-        </is>
-      </c>
+      <c r="D486" t="inlineStr"/>
       <c r="E486" t="n">
         <v>91</v>
       </c>
@@ -24157,11 +24005,7 @@
           <t>1351010101000</t>
         </is>
       </c>
-      <c r="D502" t="inlineStr">
-        <is>
-          <t>OUTORGA DIR. USO EXPLORACAO CRIACAO PROTEGIDA - INSTITUICAO CIENTIFICA TECNOLOGICA - PRINC.</t>
-        </is>
-      </c>
+      <c r="D502" t="inlineStr"/>
       <c r="E502" t="n">
         <v>60</v>
       </c>
@@ -25721,11 +25565,7 @@
           <t>1923990103000</t>
         </is>
       </c>
-      <c r="D535" t="inlineStr">
-        <is>
-          <t>OUTROS RESSARCIMENTOS - PRINC. - FORMACAO ACADEMICA NA AREA DE SAUDE</t>
-        </is>
-      </c>
+      <c r="D535" t="inlineStr"/>
       <c r="E535" t="n">
         <v>60</v>
       </c>
@@ -28261,11 +28101,7 @@
           <t>1351010101000</t>
         </is>
       </c>
-      <c r="D589" t="inlineStr">
-        <is>
-          <t>OUTORGA DIR. USO EXPLORACAO CRIACAO PROTEGIDA - INSTITUICAO CIENTIFICA TECNOLOGICA - PRINC.</t>
-        </is>
-      </c>
+      <c r="D589" t="inlineStr"/>
       <c r="E589" t="n">
         <v>60</v>
       </c>
@@ -28549,11 +28385,7 @@
           <t>1631530201000</t>
         </is>
       </c>
-      <c r="D595" t="inlineStr">
-        <is>
-          <t>SERVICOS AMBULATORIAIS - MJM</t>
-        </is>
-      </c>
+      <c r="D595" t="inlineStr"/>
       <c r="E595" t="n">
         <v>60</v>
       </c>
@@ -32425,11 +32257,7 @@
           <t>7699990101000</t>
         </is>
       </c>
-      <c r="D677" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - OUTROS SERVICOS - PRINC.</t>
-        </is>
-      </c>
+      <c r="D677" t="inlineStr"/>
       <c r="E677" t="n">
         <v>60</v>
       </c>
@@ -32845,11 +32673,7 @@
           <t>1611010129000</t>
         </is>
       </c>
-      <c r="D686" t="inlineStr">
-        <is>
-          <t>SERVICOS ADM. COMERC. GER. - PRINC. - HOSPEDAGEM E ALIMENTACAO</t>
-        </is>
-      </c>
+      <c r="D686" t="inlineStr"/>
       <c r="E686" t="n">
         <v>60</v>
       </c>
@@ -35333,11 +35157,7 @@
           <t>1911090499000</t>
         </is>
       </c>
-      <c r="D738" t="inlineStr">
-        <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D738" t="inlineStr"/>
       <c r="E738" t="n">
         <v>60</v>
       </c>
@@ -35381,11 +35201,7 @@
           <t>1911090499000</t>
         </is>
       </c>
-      <c r="D739" t="inlineStr">
-        <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D739" t="inlineStr"/>
       <c r="E739" t="n">
         <v>77</v>
       </c>
@@ -36055,7 +35871,7 @@
       </c>
       <c r="D753" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E753" t="n">
@@ -36477,7 +36293,7 @@
       </c>
       <c r="B762" t="inlineStr">
         <is>
-          <t>FUNDALEMG</t>
+          <t>FUNDHAB</t>
         </is>
       </c>
       <c r="C762" t="inlineStr">
@@ -36525,7 +36341,7 @@
       </c>
       <c r="B763" t="inlineStr">
         <is>
-          <t>FUNDALEMG</t>
+          <t>FUNDHAB</t>
         </is>
       </c>
       <c r="C763" t="inlineStr">
@@ -36573,7 +36389,7 @@
       </c>
       <c r="B764" t="inlineStr">
         <is>
-          <t>FUNDALEMG</t>
+          <t>FUNDHAB</t>
         </is>
       </c>
       <c r="C764" t="inlineStr">
@@ -37721,11 +37537,7 @@
           <t>1739990111001</t>
         </is>
       </c>
-      <c r="D789" t="inlineStr">
-        <is>
-          <t>COMERCIO E SERVICOS - DIVERSOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D789" t="inlineStr"/>
       <c r="E789" t="n">
         <v>59</v>
       </c>
@@ -38201,11 +38013,7 @@
           <t>1611030105000</t>
         </is>
       </c>
-      <c r="D799" t="inlineStr">
-        <is>
-          <t>SERVICOS REG. CERTIF. FISCALIZ. - PRINC. - INSPECAO E FISCALIZACAO</t>
-        </is>
-      </c>
+      <c r="D799" t="inlineStr"/>
       <c r="E799" t="n">
         <v>60</v>
       </c>
@@ -39305,11 +39113,7 @@
           <t>7729990127000</t>
         </is>
       </c>
-      <c r="D822" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - OUTRAS TRANSF. ESTADOS DF - PRINC. - REPASSE DO FUNDO ESPECIAL DO MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - FUNEMP</t>
-        </is>
-      </c>
+      <c r="D822" t="inlineStr"/>
       <c r="E822" t="n">
         <v>60</v>
       </c>
@@ -39835,7 +39639,7 @@
       </c>
       <c r="D833" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E833" t="n">
@@ -40361,11 +40165,7 @@
           <t>1321050101000</t>
         </is>
       </c>
-      <c r="D844" t="inlineStr">
-        <is>
-          <t>JUROS TITULOS RENDA - PRINC. - RENDIMENTO DE APLICACAO FINANCEIRA - TITULOS DE CREDITO</t>
-        </is>
-      </c>
+      <c r="D844" t="inlineStr"/>
       <c r="E844" t="n">
         <v>60</v>
       </c>
@@ -40553,11 +40353,7 @@
           <t>1911090101003</t>
         </is>
       </c>
-      <c r="D848" t="inlineStr">
-        <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - PRINC. - PPP - DIREITOS DA CIDADANIA</t>
-        </is>
-      </c>
+      <c r="D848" t="inlineStr"/>
       <c r="E848" t="n">
         <v>60</v>
       </c>
@@ -41889,11 +41685,7 @@
           <t>1219991110001</t>
         </is>
       </c>
-      <c r="D876" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D876" t="inlineStr"/>
       <c r="E876" t="n">
         <v>30</v>
       </c>
@@ -42753,11 +42545,7 @@
           <t>7219991110051</t>
         </is>
       </c>
-      <c r="D894" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D894" t="inlineStr"/>
       <c r="E894" t="n">
         <v>75</v>
       </c>
@@ -42801,11 +42589,7 @@
           <t>7219991110052</t>
         </is>
       </c>
-      <c r="D895" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D895" t="inlineStr"/>
       <c r="E895" t="n">
         <v>75</v>
       </c>
@@ -43045,11 +42829,7 @@
           <t>1999122101000</t>
         </is>
       </c>
-      <c r="D901" t="inlineStr">
-        <is>
-          <t>ONUS SUCUMBENCIA - PRINC. - HONORARIOS DE ADVOGADOS</t>
-        </is>
-      </c>
+      <c r="D901" t="inlineStr"/>
       <c r="E901" t="n">
         <v>60</v>
       </c>
@@ -44909,11 +44689,7 @@
           <t>1114501101002</t>
         </is>
       </c>
-      <c r="D942" t="inlineStr">
-        <is>
-          <t>ICMS - PRINC. - COTA PARTE ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D942" t="inlineStr"/>
       <c r="E942" t="n">
         <v>10</v>
       </c>
@@ -45101,11 +44877,7 @@
           <t>1114501201002</t>
         </is>
       </c>
-      <c r="D946" t="inlineStr">
-        <is>
-          <t>ICMS - MJM - COTA PARTE ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D946" t="inlineStr"/>
       <c r="E946" t="n">
         <v>10</v>
       </c>
@@ -47213,11 +46985,7 @@
           <t>1121010301002</t>
         </is>
       </c>
-      <c r="D990" t="inlineStr">
-        <is>
-          <t>TX. INSP. CONTR. FISC. - DA - TX. SEGURANCA PUBLICA - CORPO DE BOMBEIROS MILITAR DO ESTADO DE MINAS GERAIS - CBMMG</t>
-        </is>
-      </c>
+      <c r="D990" t="inlineStr"/>
       <c r="E990" t="n">
         <v>27</v>
       </c>
@@ -47453,11 +47221,7 @@
           <t>1121010401002</t>
         </is>
       </c>
-      <c r="D995" t="inlineStr">
-        <is>
-          <t>TX. INSP. CONTR. FISC. - DA-MJM - TX. SEGURANCA PUBLICA - CORPO DE BOMBEIROS MILITAR DO ESTADO DE MINAS GERAIS - CBMMG</t>
-        </is>
-      </c>
+      <c r="D995" t="inlineStr"/>
       <c r="E995" t="n">
         <v>27</v>
       </c>
@@ -49949,11 +49713,7 @@
           <t>1215521101000</t>
         </is>
       </c>
-      <c r="D1047" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - APOSENTADORIA</t>
-        </is>
-      </c>
+      <c r="D1047" t="inlineStr"/>
       <c r="E1047" t="n">
         <v>30</v>
       </c>
@@ -50141,11 +49901,7 @@
           <t>1219991110001</t>
         </is>
       </c>
-      <c r="D1051" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D1051" t="inlineStr"/>
       <c r="E1051" t="n">
         <v>30</v>
       </c>
@@ -50573,11 +50329,7 @@
           <t>1311020102000</t>
         </is>
       </c>
-      <c r="D1060" t="inlineStr">
-        <is>
-          <t>CONC. PERM. AUTOR. CESSAO DIR. USO BENS IMOV. PUB. - PRINC. - CESSAO DO DIREITO DE EXPLORACAO DE ESTADIOS - ARENA INDEPENDENCIA</t>
-        </is>
-      </c>
+      <c r="D1060" t="inlineStr"/>
       <c r="E1060" t="n">
         <v>15</v>
       </c>
@@ -50813,11 +50565,7 @@
           <t>1311990101000</t>
         </is>
       </c>
-      <c r="D1065" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. IMOBILIARIAS - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1065" t="inlineStr"/>
       <c r="E1065" t="n">
         <v>15</v>
       </c>
@@ -50861,11 +50609,7 @@
           <t>1311990201000</t>
         </is>
       </c>
-      <c r="D1066" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. IMOBILIARIAS - MJM</t>
-        </is>
-      </c>
+      <c r="D1066" t="inlineStr"/>
       <c r="E1066" t="n">
         <v>15</v>
       </c>
@@ -51917,11 +51661,7 @@
           <t>1321020101000</t>
         </is>
       </c>
-      <c r="D1088" t="inlineStr">
-        <is>
-          <t>REMUNERACAO DEPOSITOS ESPECIAIS - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1088" t="inlineStr"/>
       <c r="E1088" t="n">
         <v>15</v>
       </c>
@@ -51965,11 +51705,7 @@
           <t>1321050102000</t>
         </is>
       </c>
-      <c r="D1089" t="inlineStr">
-        <is>
-          <t>JUROS TITULOS RENDA - PRINC. - RENDIMENTO FINANCEIRO - ATIVO BDMG/CREDIREAL/BEMGE - SANEAMENTO SISTEMA FINANCEIRO</t>
-        </is>
-      </c>
+      <c r="D1089" t="inlineStr"/>
       <c r="E1089" t="n">
         <v>15</v>
       </c>
@@ -52637,11 +52373,7 @@
           <t>1361012101000</t>
         </is>
       </c>
-      <c r="D1103" t="inlineStr">
-        <is>
-          <t>CESSAO DIR. OPERAC. PAG. - PODER JUDICIARIO - PRINC. - FOLHA DE PESSOAL</t>
-        </is>
-      </c>
+      <c r="D1103" t="inlineStr"/>
       <c r="E1103" t="n">
         <v>60</v>
       </c>
@@ -53933,11 +53665,7 @@
           <t>1611010135000</t>
         </is>
       </c>
-      <c r="D1130" t="inlineStr">
-        <is>
-          <t>SERVICOS ADM. COMERC. GER. - PRINC. - REGISTRO ELETRONICO DE CONTRATO INTEGRAL</t>
-        </is>
-      </c>
+      <c r="D1130" t="inlineStr"/>
       <c r="E1130" t="n">
         <v>15</v>
       </c>
@@ -55229,11 +54957,7 @@
           <t>1715520101000</t>
         </is>
       </c>
-      <c r="D1157" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPLEM. UNIAO FUNDEB - VAAR - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1157" t="inlineStr"/>
       <c r="E1157" t="n">
         <v>90</v>
       </c>
@@ -55325,11 +55049,7 @@
           <t>1719620101000</t>
         </is>
       </c>
-      <c r="D1159" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO ESTADO</t>
-        </is>
-      </c>
+      <c r="D1159" t="inlineStr"/>
       <c r="E1159" t="n">
         <v>19</v>
       </c>
@@ -55373,11 +55093,7 @@
           <t>1719620102000</t>
         </is>
       </c>
-      <c r="D1160" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D1160" t="inlineStr"/>
       <c r="E1160" t="n">
         <v>20</v>
       </c>
@@ -55421,11 +55137,7 @@
           <t>1719620103000</t>
         </is>
       </c>
-      <c r="D1161" t="inlineStr">
-        <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
-        </is>
-      </c>
+      <c r="D1161" t="inlineStr"/>
       <c r="E1161" t="n">
         <v>23</v>
       </c>
@@ -55517,11 +55229,7 @@
           <t>1719990129000</t>
         </is>
       </c>
-      <c r="D1163" t="inlineStr">
-        <is>
-          <t>OUTRAS TRANSF. UNIAO ENTIDADES - AUXILIO DE COMPLEMENTACAO DO FPE - LC N 201/2023</t>
-        </is>
-      </c>
+      <c r="D1163" t="inlineStr"/>
       <c r="E1163" t="n">
         <v>15</v>
       </c>
@@ -55565,11 +55273,7 @@
           <t>1739990111001</t>
         </is>
       </c>
-      <c r="D1164" t="inlineStr">
-        <is>
-          <t>COMERCIO E SERVICOS - DIVERSOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D1164" t="inlineStr"/>
       <c r="E1164" t="n">
         <v>11</v>
       </c>
@@ -55613,11 +55317,7 @@
           <t>1741990133999</t>
         </is>
       </c>
-      <c r="D1165" t="inlineStr">
-        <is>
-          <t>ACOES ESSENCIAIS JUSTICA - OUTROS</t>
-        </is>
-      </c>
+      <c r="D1165" t="inlineStr"/>
       <c r="E1165" t="n">
         <v>60</v>
       </c>
@@ -55757,11 +55457,7 @@
           <t>1741990140999</t>
         </is>
       </c>
-      <c r="D1168" t="inlineStr">
-        <is>
-          <t>DESPORTO LAZER - OUTROS</t>
-        </is>
-      </c>
+      <c r="D1168" t="inlineStr"/>
       <c r="E1168" t="n">
         <v>11</v>
       </c>
@@ -55805,11 +55501,7 @@
           <t>1741990140999</t>
         </is>
       </c>
-      <c r="D1169" t="inlineStr">
-        <is>
-          <t>DESPORTO LAZER - OUTROS</t>
-        </is>
-      </c>
+      <c r="D1169" t="inlineStr"/>
       <c r="E1169" t="n">
         <v>59</v>
       </c>
@@ -55855,7 +55547,7 @@
       </c>
       <c r="D1170" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E1170" t="n">
@@ -55903,7 +55595,7 @@
       </c>
       <c r="D1171" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E1171" t="n">
@@ -55951,7 +55643,7 @@
       </c>
       <c r="D1172" t="inlineStr">
         <is>
-          <t>DIR. HUMANOS CIDADANIA - OUTROS</t>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
         </is>
       </c>
       <c r="E1172" t="n">
@@ -56093,11 +55785,7 @@
           <t>1751500102001</t>
         </is>
       </c>
-      <c r="D1175" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - LC FEDERAL NO 87/96 - COTA PARTE DO ESTADO</t>
-        </is>
-      </c>
+      <c r="D1175" t="inlineStr"/>
       <c r="E1175" t="n">
         <v>23</v>
       </c>
@@ -56765,11 +56453,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D1189" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D1189" t="inlineStr"/>
       <c r="E1189" t="n">
         <v>13</v>
       </c>
@@ -56813,11 +56497,7 @@
           <t>1751500109005</t>
         </is>
       </c>
-      <c r="D1190" t="inlineStr">
-        <is>
-          <t>TRANSF. RECURSOS FUNDEB - PRINC. - PARCELA ADICIONAL ICMS - FEM - EXERCICIOS ANTERIORES</t>
-        </is>
-      </c>
+      <c r="D1190" t="inlineStr"/>
       <c r="E1190" t="n">
         <v>23</v>
       </c>
@@ -56957,11 +56637,7 @@
           <t>1792010101000</t>
         </is>
       </c>
-      <c r="D1193" t="inlineStr">
-        <is>
-          <t>TRANSF. DEPOSITOS NAO IDENTIFICADOS - PRINC. - CAMPANHA DE DOACAO CORONAVIRUS</t>
-        </is>
-      </c>
+      <c r="D1193" t="inlineStr"/>
       <c r="E1193" t="n">
         <v>26</v>
       </c>
@@ -57005,11 +56681,7 @@
           <t>1792010101000</t>
         </is>
       </c>
-      <c r="D1194" t="inlineStr">
-        <is>
-          <t>TRANSF. DEPOSITOS NAO IDENTIFICADOS - PRINC. - CAMPANHA DE DOACAO CORONAVIRUS</t>
-        </is>
-      </c>
+      <c r="D1194" t="inlineStr"/>
       <c r="E1194" t="n">
         <v>46</v>
       </c>
@@ -57341,11 +57013,7 @@
           <t>1911010104001</t>
         </is>
       </c>
-      <c r="D1201" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1201" t="inlineStr"/>
       <c r="E1201" t="n">
         <v>15</v>
       </c>
@@ -57533,11 +57201,7 @@
           <t>1911010109000</t>
         </is>
       </c>
-      <c r="D1205" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - DESMONTE DE VEICULOS</t>
-        </is>
-      </c>
+      <c r="D1205" t="inlineStr"/>
       <c r="E1205" t="n">
         <v>15</v>
       </c>
@@ -57725,11 +57389,7 @@
           <t>1911010304001</t>
         </is>
       </c>
-      <c r="D1209" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISL. ESPECIFICA - DA - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1209" t="inlineStr"/>
       <c r="E1209" t="n">
         <v>15</v>
       </c>
@@ -57973,11 +57633,7 @@
       <c r="E1214" t="n">
         <v>79</v>
       </c>
-      <c r="F1214" t="inlineStr">
-        <is>
-          <t>CONTRIBUICAO PATRONAL PARA O FUNPREV</t>
-        </is>
-      </c>
+      <c r="F1214" t="inlineStr"/>
       <c r="G1214" t="n">
         <v>0</v>
       </c>
@@ -58205,11 +57861,7 @@
           <t>1911132101000</t>
         </is>
       </c>
-      <c r="D1219" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISLACAO ANTICORRUPCAO ACORDOS LENIENCIA - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1219" t="inlineStr"/>
       <c r="E1219" t="n">
         <v>15</v>
       </c>
@@ -58349,11 +58001,7 @@
           <t>1921030101000</t>
         </is>
       </c>
-      <c r="D1222" t="inlineStr">
-        <is>
-          <t>INDENIZACAO SINISTRO - PRINC.</t>
-        </is>
-      </c>
+      <c r="D1222" t="inlineStr"/>
       <c r="E1222" t="n">
         <v>60</v>
       </c>
@@ -59021,11 +58669,7 @@
           <t>1922063299000</t>
         </is>
       </c>
-      <c r="D1236" t="inlineStr">
-        <is>
-          <t>RESTITUICAO DESPESAS PRIMARIAS EXERCICIOS ANTERIORES - MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D1236" t="inlineStr"/>
       <c r="E1236" t="n">
         <v>25</v>
       </c>
@@ -60029,11 +59673,7 @@
           <t>1922990399000</t>
         </is>
       </c>
-      <c r="D1257" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D1257" t="inlineStr"/>
       <c r="E1257" t="n">
         <v>60</v>
       </c>
@@ -60077,11 +59717,7 @@
           <t>1922990499000</t>
         </is>
       </c>
-      <c r="D1258" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - DA-MJM - DEMAIS</t>
-        </is>
-      </c>
+      <c r="D1258" t="inlineStr"/>
       <c r="E1258" t="n">
         <v>60</v>
       </c>
@@ -60365,11 +60001,7 @@
           <t>1999992101000</t>
         </is>
       </c>
-      <c r="D1264" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - RECURSOS DE DEPOSITOS JUDICIAIS</t>
-        </is>
-      </c>
+      <c r="D1264" t="inlineStr"/>
       <c r="E1264" t="n">
         <v>23</v>
       </c>
@@ -60605,11 +60237,7 @@
           <t>1999992113000</t>
         </is>
       </c>
-      <c r="D1269" t="inlineStr">
-        <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - CONVERSAO EM RENDA DE VALORES PENHORADOS EM ACOES JUDICIAIS</t>
-        </is>
-      </c>
+      <c r="D1269" t="inlineStr"/>
       <c r="E1269" t="n">
         <v>15</v>
       </c>
@@ -61373,11 +61001,7 @@
           <t>2211020104000</t>
         </is>
       </c>
-      <c r="D1285" t="inlineStr">
-        <is>
-          <t>ALIEN. TITULOS VALORES MOBIL. APLIC. CONGEN. PERMANENTES - PRINC. - MINAS CAIXA</t>
-        </is>
-      </c>
+      <c r="D1285" t="inlineStr"/>
       <c r="E1285" t="n">
         <v>48</v>
       </c>
@@ -61421,11 +61045,7 @@
           <t>2211020105000</t>
         </is>
       </c>
-      <c r="D1286" t="inlineStr">
-        <is>
-          <t>ALIEN. TITULOS VALORES MOBIL. APLIC. CONGEN. PERMANENTES - PRINC. - SANEAMENTO DO SISTEMA FINANCEIRO - CREDIREAL/BEMGE</t>
-        </is>
-      </c>
+      <c r="D1286" t="inlineStr"/>
       <c r="E1286" t="n">
         <v>48</v>
       </c>
@@ -61999,7 +61619,7 @@
       </c>
       <c r="D1298" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - DEMAIS RECURSOS</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
         </is>
       </c>
       <c r="E1298" t="n">
@@ -62045,11 +61665,7 @@
           <t>2999990104000</t>
         </is>
       </c>
-      <c r="D1299" t="inlineStr">
-        <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - ACORDO JUDICIAL DE REPARACAO INTEGRAL E DEFINITIVA</t>
-        </is>
-      </c>
+      <c r="D1299" t="inlineStr"/>
       <c r="E1299" t="n">
         <v>80</v>
       </c>
@@ -62093,11 +61709,7 @@
           <t>7215531102000</t>
         </is>
       </c>
-      <c r="D1300" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D1300" t="inlineStr"/>
       <c r="E1300" t="n">
         <v>75</v>
       </c>
@@ -62141,11 +61753,7 @@
           <t>7215531103000</t>
         </is>
       </c>
-      <c r="D1301" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - APOSENTADORIA</t>
-        </is>
-      </c>
+      <c r="D1301" t="inlineStr"/>
       <c r="E1301" t="n">
         <v>75</v>
       </c>
@@ -62189,11 +61797,7 @@
           <t>7215532102000</t>
         </is>
       </c>
-      <c r="D1302" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - PENSAO</t>
-        </is>
-      </c>
+      <c r="D1302" t="inlineStr"/>
       <c r="E1302" t="n">
         <v>75</v>
       </c>
@@ -62237,11 +61841,7 @@
           <t>7215532103000</t>
         </is>
       </c>
-      <c r="D1303" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - APOSENTADORIA</t>
-        </is>
-      </c>
+      <c r="D1303" t="inlineStr"/>
       <c r="E1303" t="n">
         <v>75</v>
       </c>
@@ -62285,11 +61885,7 @@
           <t>7219991110051</t>
         </is>
       </c>
-      <c r="D1304" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - ATIVO</t>
-        </is>
-      </c>
+      <c r="D1304" t="inlineStr"/>
       <c r="E1304" t="n">
         <v>75</v>
       </c>
@@ -62333,11 +61929,7 @@
           <t>7219991110052</t>
         </is>
       </c>
-      <c r="D1305" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRONAL MILITAR APOSENTADORIA - INATIVO</t>
-        </is>
-      </c>
+      <c r="D1305" t="inlineStr"/>
       <c r="E1305" t="n">
         <v>75</v>
       </c>
@@ -62957,11 +62549,7 @@
           <t>9114501101002</t>
         </is>
       </c>
-      <c r="D1318" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DO ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1318" t="inlineStr"/>
       <c r="E1318" t="n">
         <v>10</v>
       </c>
@@ -63101,11 +62689,7 @@
           <t>9114501201002</t>
         </is>
       </c>
-      <c r="D1321" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DO ESTADO - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1321" t="inlineStr"/>
       <c r="E1321" t="n">
         <v>10</v>
       </c>
@@ -63773,11 +63357,7 @@
           <t>9719620102000</t>
         </is>
       </c>
-      <c r="D1335" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
-        </is>
-      </c>
+      <c r="D1335" t="inlineStr"/>
       <c r="E1335" t="n">
         <v>20</v>
       </c>
@@ -63821,11 +63401,7 @@
           <t>9719620103000</t>
         </is>
       </c>
-      <c r="D1336" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
-        </is>
-      </c>
+      <c r="D1336" t="inlineStr"/>
       <c r="E1336" t="n">
         <v>23</v>
       </c>
@@ -63965,11 +63541,7 @@
           <t>9911010104001</t>
         </is>
       </c>
-      <c r="D1339" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - MULTAS LEGISL. ESPECIFICA - PRINC. - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1339" t="inlineStr"/>
       <c r="E1339" t="n">
         <v>15</v>
       </c>
@@ -64013,11 +63585,7 @@
           <t>9911010304001</t>
         </is>
       </c>
-      <c r="D1340" t="inlineStr">
-        <is>
-          <t>DEDUCAO REC. - MULTAS LEGISL. ESPECIFICA - DA - MULTA ISOLADA OBRIG. ACESSORIA - CESSAO DE DIREITOS CREDITORIOS - LEI ESTADUAL NO 19.266/10</t>
-        </is>
-      </c>
+      <c r="D1340" t="inlineStr"/>
       <c r="E1340" t="n">
         <v>15</v>
       </c>

</xml_diff>